<commit_message>
faster Mongolia cold stations min max retrieve
</commit_message>
<xml_diff>
--- a/气象/全国所有站点(国家站)全年及各月极端高低温.xlsx
+++ b/气象/全国所有站点(国家站)全年及各月极端高低温.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\文档\GIT SYNC\default\气象\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BEB8FC-CE52-432A-AB95-A1D399738BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB3DA6A-746F-4212-8EFC-F73C8CEA9D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{172DB64A-34A6-4C2C-B594-936105A71AD1}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{172DB64A-34A6-4C2C-B594-936105A71AD1}"/>
   </bookViews>
   <sheets>
     <sheet name="国家站极端温度" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="各省最低温" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">国家站极端温度!$A$1:$H$2470</definedName>
@@ -8525,7 +8525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6EE9646-D37D-425D-B0F8-150E85433B03}">
   <dimension ref="A1:H2470"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1430" workbookViewId="0">
+    <sheetView topLeftCell="A1430" workbookViewId="0">
       <selection activeCell="L1439" sqref="L1439"/>
     </sheetView>
   </sheetViews>
@@ -80181,8 +80181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8CD8AC-0906-4D8B-9742-1E6BA5AF7DE6}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>

</xml_diff>